<commit_message>
excelImport: FieldCastException not resolved
</commit_message>
<xml_diff>
--- a/src/main/resources/BankBranch.xlsx
+++ b/src/main/resources/BankBranch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Branch Code</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Tongi</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,68 +400,116 @@
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D2">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D3">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D4">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D5">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D6">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1006</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D7">
+        <v>90.414381000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1007</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
+      </c>
+      <c r="C8">
+        <v>23.833389199999999</v>
+      </c>
+      <c r="D8">
+        <v>90.414381000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>